<commit_message>
finished set by column name
</commit_message>
<xml_diff>
--- a/forms/fisher_form.xlsx
+++ b/forms/fisher_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob\Desktop\Autofill 1.0.1\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba3bd2985b379b5a/Documents/Autofill/forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616BE047-885E-43DD-9B2E-2E8B01E76CF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616BE047-885E-43DD-9B2E-2E8B01E76CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2850" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Submission Details" sheetId="3" r:id="rId1"/>
@@ -2001,10 +2001,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:DI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CZ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="DB9" sqref="DB9"/>
+      <selection pane="bottomLeft" activeCell="CZ1" sqref="CZ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,9 +2657,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BM2"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="BJ1" sqref="BJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>